<commit_message>
Finish off round tube options (all 154)
</commit_message>
<xml_diff>
--- a/RoundTube_Options.xlsx
+++ b/RoundTube_Options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimmer\OneDrive - Rose-Hulman Institute of Technology\Documents\!! RHIT Fall 2021-22\EM204\EM204_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E33E50E-0297-4ECB-82E2-64F8DF519F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEF562B-52B9-4359-AF83-66930693CD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{94F3ECEF-463D-4A3F-B5B9-6A9324BF671F}"/>
   </bookViews>
@@ -49,8 +49,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,22 +403,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5547D6A7-4251-48A0-B41D-4C97424E1C73}">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1614,300 +1623,655 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>0.125</v>
+      </c>
       <c r="C102">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1.625</v>
+      </c>
+      <c r="B103">
+        <v>0.125</v>
+      </c>
       <c r="C103">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.375</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1.5</v>
+      </c>
+      <c r="B104">
+        <v>0.375</v>
+      </c>
       <c r="C104">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>0.1875</v>
+      </c>
       <c r="C105">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106">
+        <v>0.25</v>
+      </c>
       <c r="C106">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>0.1875</v>
+      </c>
       <c r="C107">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.625</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2.5</v>
+      </c>
+      <c r="B108">
+        <v>0.25</v>
+      </c>
       <c r="C108">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2.75</v>
+      </c>
+      <c r="B109">
+        <v>0.25</v>
+      </c>
       <c r="C109">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>4.5</v>
+      </c>
+      <c r="B110">
+        <v>0.125</v>
+      </c>
       <c r="C110">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C111">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1.375</v>
+      </c>
+      <c r="B112">
+        <v>0.25</v>
+      </c>
       <c r="C112">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>5</v>
+      </c>
+      <c r="B113">
+        <v>0.125</v>
+      </c>
       <c r="C113">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>3</v>
+      </c>
+      <c r="B114">
+        <v>0.25</v>
+      </c>
       <c r="C114">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>8</v>
+      </c>
+      <c r="B115">
+        <v>0.125</v>
+      </c>
       <c r="C115">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>3.5</v>
+      </c>
+      <c r="B116">
+        <v>0.1875</v>
+      </c>
       <c r="C116">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2.75</v>
+      </c>
+      <c r="B117">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C117">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>0.75</v>
+      </c>
       <c r="C118">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>3.5</v>
+      </c>
+      <c r="B119">
+        <v>0.25</v>
+      </c>
       <c r="C119">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2.5</v>
+      </c>
+      <c r="B120">
+        <v>0.375</v>
+      </c>
       <c r="C120">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1.125</v>
+      </c>
+      <c r="B121">
+        <v>0.25</v>
+      </c>
       <c r="C121">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>6</v>
+      </c>
+      <c r="B122">
+        <v>0.125</v>
+      </c>
       <c r="C122">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2.5</v>
+      </c>
+      <c r="B123">
+        <v>0.5</v>
+      </c>
       <c r="C123">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>0.1875</v>
+      </c>
       <c r="C124">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.625</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="B125">
+        <v>0.375</v>
+      </c>
       <c r="C125">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>3.5</v>
+      </c>
+      <c r="B126">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C126">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127">
+        <v>0.1875</v>
+      </c>
       <c r="C127">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>0.25</v>
+      </c>
       <c r="C128">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>7</v>
+      </c>
+      <c r="B129">
+        <v>0.125</v>
+      </c>
       <c r="C129">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130">
+        <v>0.25</v>
+      </c>
       <c r="C130">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>4.5</v>
+      </c>
+      <c r="B131">
+        <v>0.25</v>
+      </c>
       <c r="C131">
-        <f t="shared" ref="C131:C150" si="2">A131-2*B131</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C131:C155" si="2">A131-2*B131</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C132">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>5</v>
+      </c>
+      <c r="B133">
+        <v>6.5000000000000002E-2</v>
+      </c>
       <c r="C133">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4.87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>6</v>
+      </c>
+      <c r="B134">
+        <v>0.25</v>
+      </c>
       <c r="C134">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>6</v>
+      </c>
+      <c r="B135">
+        <v>0.1875</v>
+      </c>
       <c r="C135">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>3.5</v>
+      </c>
+      <c r="B136">
+        <v>0.5</v>
+      </c>
       <c r="C136">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>3.5</v>
+      </c>
+      <c r="B137">
+        <v>0.375</v>
+      </c>
       <c r="C137">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>5.5</v>
+      </c>
+      <c r="B138">
+        <v>0.25</v>
+      </c>
       <c r="C138">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>4.5</v>
+      </c>
+      <c r="B139">
+        <v>0.375</v>
+      </c>
       <c r="C139">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>4</v>
+      </c>
+      <c r="B140">
+        <v>0.5</v>
+      </c>
       <c r="C140">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>7</v>
+      </c>
+      <c r="B141">
+        <v>0.25</v>
+      </c>
       <c r="C141">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>4.25</v>
+      </c>
+      <c r="B142">
+        <v>0.5</v>
+      </c>
       <c r="C142">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>6</v>
+      </c>
+      <c r="B143">
+        <v>0.5</v>
+      </c>
       <c r="C143">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>4.5</v>
+      </c>
+      <c r="B144">
+        <v>0.5</v>
+      </c>
       <c r="C144">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>4.5</v>
+      </c>
+      <c r="B145">
+        <v>0.75</v>
+      </c>
       <c r="C145">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>5</v>
+      </c>
+      <c r="B146">
+        <v>0.5</v>
+      </c>
       <c r="C146">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>7</v>
+      </c>
+      <c r="B147">
+        <v>0.25</v>
+      </c>
       <c r="C147">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>7</v>
+      </c>
+      <c r="B148">
+        <v>0.5</v>
+      </c>
       <c r="C148">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>8</v>
+      </c>
+      <c r="B149">
+        <v>0.5</v>
+      </c>
       <c r="C149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>12</v>
+      </c>
+      <c r="B150">
+        <v>0.25</v>
+      </c>
       <c r="C150">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>7.5</v>
+      </c>
+      <c r="B151">
+        <v>0.5</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>9</v>
+      </c>
+      <c r="B152">
+        <v>0.5</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>9</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>8</v>
+      </c>
+      <c r="B154">
+        <v>1.5</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>8.5</v>
+      </c>
+      <c r="B155">
+        <v>0.5</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with round bar options
</commit_message>
<xml_diff>
--- a/RoundTube_Options.xlsx
+++ b/RoundTube_Options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimmer\OneDrive - Rose-Hulman Institute of Technology\Documents\!! RHIT Fall 2021-22\EM204\EM204_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEF562B-52B9-4359-AF83-66930693CD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1380D9-17EB-4FD8-9401-9C447E24D035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{94F3ECEF-463D-4A3F-B5B9-6A9324BF671F}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Messed up measurement in port over
</commit_message>
<xml_diff>
--- a/RoundTube_Options.xlsx
+++ b/RoundTube_Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimmer\OneDrive - Rose-Hulman Institute of Technology\Documents\!! RHIT Fall 2021-22\EM204\EM204_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB71A44-BAC0-457E-A86E-9E10A6E9B3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1B21C84-855A-4A4A-B59F-A85965BDCB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1260" windowWidth="21600" windowHeight="11325" xr2:uid="{94F3ECEF-463D-4A3F-B5B9-6A9324BF671F}"/>
+    <workbookView xWindow="6570" yWindow="2970" windowWidth="21600" windowHeight="11325" xr2:uid="{94F3ECEF-463D-4A3F-B5B9-6A9324BF671F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5547D6A7-4251-48A0-B41D-4C97424E1C73}">
   <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,85 +2058,85 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140">
+      <c r="A140" s="1">
+        <v>8</v>
+      </c>
+      <c r="B140" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C140" s="1">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="B141" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C141" s="1">
+        <f t="shared" si="2"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>6</v>
+      </c>
+      <c r="B142" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C142" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B143" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C143" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B144" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C144" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>5</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C145" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
         <v>7</v>
       </c>
-      <c r="B140">
-        <v>0.25</v>
-      </c>
-      <c r="C140">
-        <f t="shared" si="2"/>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>4.25</v>
-      </c>
-      <c r="B141">
-        <v>0.5</v>
-      </c>
-      <c r="C141">
-        <f t="shared" si="2"/>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>6</v>
-      </c>
-      <c r="B142">
-        <v>0.5</v>
-      </c>
-      <c r="C142">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>4.5</v>
-      </c>
-      <c r="B143">
-        <v>0.5</v>
-      </c>
-      <c r="C143">
-        <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>4.5</v>
-      </c>
-      <c r="B144">
-        <v>0.75</v>
-      </c>
-      <c r="C144">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>5</v>
-      </c>
-      <c r="B145">
-        <v>0.5</v>
-      </c>
-      <c r="C145">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>7</v>
-      </c>
-      <c r="B146">
-        <v>0.25</v>
-      </c>
-      <c r="C146">
+      <c r="B146" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C146" s="1">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>

</xml_diff>